<commit_message>
refactor: put all router and ssg logic in spa-core
</commit_message>
<xml_diff>
--- a/public/data/db-source/evolution.xlsx
+++ b/public/data/db-source/evolution.xlsx
@@ -311,6 +311,15 @@
   </si>
   <si>
     <t>1706239962</t>
+  </si>
+  <si>
+    <t>sensible_data</t>
+  </si>
+  <si>
+    <t>Les données sensibles sont des catégories particulières de données personnelles qui révèlent des informations hautement confidentielles, comme l'origine raciale ou ethnique, les opinions politiques, les croyances religieuses, la santé, la vie sexuelle, ou les données biométriques. Leur traitement est soumis à des règles strictes pour éviter toute discrimination ou atteinte à la vie privée.</t>
+  </si>
+  <si>
+    <t>Les données 2 sensibles sont des catégories particulières de données personnelles qui révèlent des informations hautement confidentielles, comme l'origine raciale ou ethnique, les opinions politiques, les croyances religieuses, la santé, la vie sexuelle, ou les données biométriques. Leur traitement est soumis à des règles strictes pour éviter toute discrimination ou atteinte à la vie privée.</t>
   </si>
 </sst>
 </file>
@@ -1449,6 +1458,29 @@
         <v>99</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55">
+        <v>1760952632</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" t="s">
+        <v>100</v>
+      </c>
+      <c r="F55" t="s">
+        <v>40</v>
+      </c>
+      <c r="G55" t="s">
+        <v>101</v>
+      </c>
+      <c r="H55" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: put all router and ssg logic in spa-core (#44)
</commit_message>
<xml_diff>
--- a/public/data/db-source/evolution.xlsx
+++ b/public/data/db-source/evolution.xlsx
@@ -311,6 +311,15 @@
   </si>
   <si>
     <t>1706239962</t>
+  </si>
+  <si>
+    <t>sensible_data</t>
+  </si>
+  <si>
+    <t>Les données sensibles sont des catégories particulières de données personnelles qui révèlent des informations hautement confidentielles, comme l'origine raciale ou ethnique, les opinions politiques, les croyances religieuses, la santé, la vie sexuelle, ou les données biométriques. Leur traitement est soumis à des règles strictes pour éviter toute discrimination ou atteinte à la vie privée.</t>
+  </si>
+  <si>
+    <t>Les données 2 sensibles sont des catégories particulières de données personnelles qui révèlent des informations hautement confidentielles, comme l'origine raciale ou ethnique, les opinions politiques, les croyances religieuses, la santé, la vie sexuelle, ou les données biométriques. Leur traitement est soumis à des règles strictes pour éviter toute discrimination ou atteinte à la vie privée.</t>
   </si>
 </sst>
 </file>
@@ -1449,6 +1458,29 @@
         <v>99</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55">
+        <v>1760952632</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" t="s">
+        <v>100</v>
+      </c>
+      <c r="F55" t="s">
+        <v>40</v>
+      </c>
+      <c r="G55" t="s">
+        <v>101</v>
+      </c>
+      <c r="H55" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add: json schema, openapi and redoc
</commit_message>
<xml_diff>
--- a/public/data/db-source/evolution.xlsx
+++ b/public/data/db-source/evolution.xlsx
@@ -2858,6 +2858,12 @@
   </si>
   <si>
     <t>dep_sante___variable_550</t>
+  </si>
+  <si>
+    <t>Images aériennes sous partie 2</t>
+  </si>
+  <si>
+    <t>Images aériennes sous partie 2.1</t>
   </si>
 </sst>
 </file>
@@ -16029,6 +16035,29 @@
         <v>948</v>
       </c>
     </row>
+    <row r="889">
+      <c r="A889">
+        <v>1761859124</v>
+      </c>
+      <c r="B889" t="s">
+        <v>9</v>
+      </c>
+      <c r="C889" t="s">
+        <v>81</v>
+      </c>
+      <c r="D889" t="s">
+        <v>83</v>
+      </c>
+      <c r="F889" t="s">
+        <v>8</v>
+      </c>
+      <c r="G889" t="s">
+        <v>949</v>
+      </c>
+      <c r="H889" t="s">
+        <v>950</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add: json schema, openapi and redoc (#51)
* fix: update last modification timestamps in __table__.json and __table__.json.js

* add: json schema, openapi and redoc
</commit_message>
<xml_diff>
--- a/public/data/db-source/evolution.xlsx
+++ b/public/data/db-source/evolution.xlsx
@@ -2858,6 +2858,12 @@
   </si>
   <si>
     <t>dep_sante___variable_550</t>
+  </si>
+  <si>
+    <t>Images aériennes sous partie 2</t>
+  </si>
+  <si>
+    <t>Images aériennes sous partie 2.1</t>
   </si>
 </sst>
 </file>
@@ -16029,6 +16035,29 @@
         <v>948</v>
       </c>
     </row>
+    <row r="889">
+      <c r="A889">
+        <v>1761859124</v>
+      </c>
+      <c r="B889" t="s">
+        <v>9</v>
+      </c>
+      <c r="C889" t="s">
+        <v>81</v>
+      </c>
+      <c r="D889" t="s">
+        <v>83</v>
+      </c>
+      <c r="F889" t="s">
+        <v>8</v>
+      </c>
+      <c r="G889" t="s">
+        <v>949</v>
+      </c>
+      <c r="H889" t="s">
+        <v>950</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: link to new variable id for freq demo data
</commit_message>
<xml_diff>
--- a/public/data/db-source/evolution.xlsx
+++ b/public/data/db-source/evolution.xlsx
@@ -9542,6 +9542,75 @@
   </si>
   <si>
     <t>dataset/accident_route.xlsx</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_1</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_2</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_3</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_4</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_5</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_6</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_7</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_8</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_9</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_10</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_11</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_12</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_13</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_14</t>
+  </si>
+  <si>
+    <t>pop_region__type_region---urbaine</t>
+  </si>
+  <si>
+    <t>urbaine</t>
+  </si>
+  <si>
+    <t>pop_region__type_region---priurbaine</t>
+  </si>
+  <si>
+    <t>périurbaine</t>
+  </si>
+  <si>
+    <t>pop_region__type_region---rurale</t>
+  </si>
+  <si>
+    <t>rurale</t>
+  </si>
+  <si>
+    <t>pop_region__type_region---montagne</t>
+  </si>
+  <si>
+    <t>montagne</t>
   </si>
 </sst>
 </file>
@@ -76773,6 +76842,686 @@
         <v>1501</v>
       </c>
     </row>
+    <row r="3676">
+      <c r="A3676">
+        <v>1765633001</v>
+      </c>
+      <c r="B3676" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3676" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3676" t="s">
+        <v>3177</v>
+      </c>
+      <c r="E3676" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3676" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3677">
+      <c r="A3677">
+        <v>1765633001</v>
+      </c>
+      <c r="B3677" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3677" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3677" t="s">
+        <v>3178</v>
+      </c>
+      <c r="E3677" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3677" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3678">
+      <c r="A3678">
+        <v>1765633001</v>
+      </c>
+      <c r="B3678" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3678" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3678" t="s">
+        <v>3179</v>
+      </c>
+      <c r="E3678" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3678" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3679">
+      <c r="A3679">
+        <v>1765633001</v>
+      </c>
+      <c r="B3679" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3679" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3679" t="s">
+        <v>3180</v>
+      </c>
+      <c r="E3679" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3679" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3680">
+      <c r="A3680">
+        <v>1765633001</v>
+      </c>
+      <c r="B3680" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3680" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3680" t="s">
+        <v>3181</v>
+      </c>
+      <c r="E3680" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3680" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3681">
+      <c r="A3681">
+        <v>1765633001</v>
+      </c>
+      <c r="B3681" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3681" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3681" t="s">
+        <v>3182</v>
+      </c>
+      <c r="E3681" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3681" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3682">
+      <c r="A3682">
+        <v>1765633001</v>
+      </c>
+      <c r="B3682" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3682" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3682" t="s">
+        <v>3183</v>
+      </c>
+      <c r="E3682" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3682" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3683">
+      <c r="A3683">
+        <v>1765633001</v>
+      </c>
+      <c r="B3683" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3683" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3683" t="s">
+        <v>3184</v>
+      </c>
+      <c r="E3683" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3683" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3684">
+      <c r="A3684">
+        <v>1765633001</v>
+      </c>
+      <c r="B3684" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3684" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3684" t="s">
+        <v>3185</v>
+      </c>
+      <c r="E3684" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3684" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3685">
+      <c r="A3685">
+        <v>1765633001</v>
+      </c>
+      <c r="B3685" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3685" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3685" t="s">
+        <v>3186</v>
+      </c>
+      <c r="E3685" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3685" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3686">
+      <c r="A3686">
+        <v>1765633001</v>
+      </c>
+      <c r="B3686" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3686" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3686" t="s">
+        <v>3187</v>
+      </c>
+      <c r="E3686" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3686" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3687">
+      <c r="A3687">
+        <v>1765633001</v>
+      </c>
+      <c r="B3687" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3687" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3687" t="s">
+        <v>3188</v>
+      </c>
+      <c r="E3687" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3687" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3688">
+      <c r="A3688">
+        <v>1765633001</v>
+      </c>
+      <c r="B3688" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3688" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3688" t="s">
+        <v>3189</v>
+      </c>
+      <c r="E3688" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3688" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3689">
+      <c r="A3689">
+        <v>1765633001</v>
+      </c>
+      <c r="B3689" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3689" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3689" t="s">
+        <v>3190</v>
+      </c>
+      <c r="E3689" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3689" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3690">
+      <c r="A3690">
+        <v>1765633001</v>
+      </c>
+      <c r="B3690" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3690" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3690" t="s">
+        <v>3191</v>
+      </c>
+      <c r="E3690" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3690" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3691">
+      <c r="A3691">
+        <v>1765633001</v>
+      </c>
+      <c r="B3691" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3691" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3691" t="s">
+        <v>3192</v>
+      </c>
+      <c r="E3691" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I3691" t="s">
+        <v>3193</v>
+      </c>
+    </row>
+    <row r="3692">
+      <c r="A3692">
+        <v>1765633001</v>
+      </c>
+      <c r="B3692" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3692" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3692" t="s">
+        <v>3194</v>
+      </c>
+      <c r="E3692" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I3692" t="s">
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="3693">
+      <c r="A3693">
+        <v>1765633001</v>
+      </c>
+      <c r="B3693" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3693" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3693" t="s">
+        <v>3196</v>
+      </c>
+      <c r="E3693" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I3693" t="s">
+        <v>3197</v>
+      </c>
+    </row>
+    <row r="3694">
+      <c r="A3694">
+        <v>1765633001</v>
+      </c>
+      <c r="B3694" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3694" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3694" t="s">
+        <v>3198</v>
+      </c>
+      <c r="E3694" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I3694" t="s">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="3695">
+      <c r="A3695">
+        <v>1765633001</v>
+      </c>
+      <c r="B3695" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3695" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3695" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3695" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3695" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3696">
+      <c r="A3696">
+        <v>1765633001</v>
+      </c>
+      <c r="B3696" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3696" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3696" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3696" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3696" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3697">
+      <c r="A3697">
+        <v>1765633001</v>
+      </c>
+      <c r="B3697" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3697" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3697" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3697" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3697" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3698">
+      <c r="A3698">
+        <v>1765633001</v>
+      </c>
+      <c r="B3698" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3698" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3698" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3698" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3698" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3699">
+      <c r="A3699">
+        <v>1765633001</v>
+      </c>
+      <c r="B3699" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3699" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3699" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3699" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3699" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3700">
+      <c r="A3700">
+        <v>1765633001</v>
+      </c>
+      <c r="B3700" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3700" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3700" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3700" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3700" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3701">
+      <c r="A3701">
+        <v>1765633001</v>
+      </c>
+      <c r="B3701" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3701" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3701" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3701" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3701" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3702">
+      <c r="A3702">
+        <v>1765633001</v>
+      </c>
+      <c r="B3702" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3702" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3702" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3702" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3702" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3703">
+      <c r="A3703">
+        <v>1765633001</v>
+      </c>
+      <c r="B3703" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3703" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3703" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3703" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3703" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3704">
+      <c r="A3704">
+        <v>1765633001</v>
+      </c>
+      <c r="B3704" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3704" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3704" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3704" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3704" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3705">
+      <c r="A3705">
+        <v>1765633001</v>
+      </c>
+      <c r="B3705" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3705" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3705" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3705" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3705" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3706">
+      <c r="A3706">
+        <v>1765633001</v>
+      </c>
+      <c r="B3706" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3706" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3706" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3706" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3706" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3707">
+      <c r="A3707">
+        <v>1765633001</v>
+      </c>
+      <c r="B3707" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3707" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3707" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3707" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3707" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3708">
+      <c r="A3708">
+        <v>1765633001</v>
+      </c>
+      <c r="B3708" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3708" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3708" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3708" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3708" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3709">
+      <c r="A3709">
+        <v>1765633001</v>
+      </c>
+      <c r="B3709" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3709" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3709" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3709" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3709" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: link to new variable id for freq demo data (#77)
</commit_message>
<xml_diff>
--- a/public/data/db-source/evolution.xlsx
+++ b/public/data/db-source/evolution.xlsx
@@ -9542,6 +9542,75 @@
   </si>
   <si>
     <t>dataset/accident_route.xlsx</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_1</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_2</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_3</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_4</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_5</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_6</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_7</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_8</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_9</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_10</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_11</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_12</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_13</t>
+  </si>
+  <si>
+    <t>pop_region__population_totale---value_14</t>
+  </si>
+  <si>
+    <t>pop_region__type_region---urbaine</t>
+  </si>
+  <si>
+    <t>urbaine</t>
+  </si>
+  <si>
+    <t>pop_region__type_region---priurbaine</t>
+  </si>
+  <si>
+    <t>périurbaine</t>
+  </si>
+  <si>
+    <t>pop_region__type_region---rurale</t>
+  </si>
+  <si>
+    <t>rurale</t>
+  </si>
+  <si>
+    <t>pop_region__type_region---montagne</t>
+  </si>
+  <si>
+    <t>montagne</t>
   </si>
 </sst>
 </file>
@@ -76773,6 +76842,686 @@
         <v>1501</v>
       </c>
     </row>
+    <row r="3676">
+      <c r="A3676">
+        <v>1765633001</v>
+      </c>
+      <c r="B3676" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3676" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3676" t="s">
+        <v>3177</v>
+      </c>
+      <c r="E3676" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3676" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3677">
+      <c r="A3677">
+        <v>1765633001</v>
+      </c>
+      <c r="B3677" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3677" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3677" t="s">
+        <v>3178</v>
+      </c>
+      <c r="E3677" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3677" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3678">
+      <c r="A3678">
+        <v>1765633001</v>
+      </c>
+      <c r="B3678" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3678" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3678" t="s">
+        <v>3179</v>
+      </c>
+      <c r="E3678" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3678" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3679">
+      <c r="A3679">
+        <v>1765633001</v>
+      </c>
+      <c r="B3679" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3679" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3679" t="s">
+        <v>3180</v>
+      </c>
+      <c r="E3679" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3679" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3680">
+      <c r="A3680">
+        <v>1765633001</v>
+      </c>
+      <c r="B3680" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3680" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3680" t="s">
+        <v>3181</v>
+      </c>
+      <c r="E3680" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3680" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3681">
+      <c r="A3681">
+        <v>1765633001</v>
+      </c>
+      <c r="B3681" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3681" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3681" t="s">
+        <v>3182</v>
+      </c>
+      <c r="E3681" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3681" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3682">
+      <c r="A3682">
+        <v>1765633001</v>
+      </c>
+      <c r="B3682" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3682" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3682" t="s">
+        <v>3183</v>
+      </c>
+      <c r="E3682" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3682" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3683">
+      <c r="A3683">
+        <v>1765633001</v>
+      </c>
+      <c r="B3683" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3683" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3683" t="s">
+        <v>3184</v>
+      </c>
+      <c r="E3683" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3683" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3684">
+      <c r="A3684">
+        <v>1765633001</v>
+      </c>
+      <c r="B3684" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3684" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3684" t="s">
+        <v>3185</v>
+      </c>
+      <c r="E3684" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3684" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3685">
+      <c r="A3685">
+        <v>1765633001</v>
+      </c>
+      <c r="B3685" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3685" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3685" t="s">
+        <v>3186</v>
+      </c>
+      <c r="E3685" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3685" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3686">
+      <c r="A3686">
+        <v>1765633001</v>
+      </c>
+      <c r="B3686" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3686" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3686" t="s">
+        <v>3187</v>
+      </c>
+      <c r="E3686" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3686" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3687">
+      <c r="A3687">
+        <v>1765633001</v>
+      </c>
+      <c r="B3687" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3687" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3687" t="s">
+        <v>3188</v>
+      </c>
+      <c r="E3687" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3687" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3688">
+      <c r="A3688">
+        <v>1765633001</v>
+      </c>
+      <c r="B3688" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3688" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3688" t="s">
+        <v>3189</v>
+      </c>
+      <c r="E3688" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3688" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3689">
+      <c r="A3689">
+        <v>1765633001</v>
+      </c>
+      <c r="B3689" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3689" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3689" t="s">
+        <v>3190</v>
+      </c>
+      <c r="E3689" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3689" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3690">
+      <c r="A3690">
+        <v>1765633001</v>
+      </c>
+      <c r="B3690" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3690" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3690" t="s">
+        <v>3191</v>
+      </c>
+      <c r="E3690" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I3690" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3691">
+      <c r="A3691">
+        <v>1765633001</v>
+      </c>
+      <c r="B3691" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3691" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3691" t="s">
+        <v>3192</v>
+      </c>
+      <c r="E3691" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I3691" t="s">
+        <v>3193</v>
+      </c>
+    </row>
+    <row r="3692">
+      <c r="A3692">
+        <v>1765633001</v>
+      </c>
+      <c r="B3692" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3692" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3692" t="s">
+        <v>3194</v>
+      </c>
+      <c r="E3692" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I3692" t="s">
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="3693">
+      <c r="A3693">
+        <v>1765633001</v>
+      </c>
+      <c r="B3693" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3693" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3693" t="s">
+        <v>3196</v>
+      </c>
+      <c r="E3693" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I3693" t="s">
+        <v>3197</v>
+      </c>
+    </row>
+    <row r="3694">
+      <c r="A3694">
+        <v>1765633001</v>
+      </c>
+      <c r="B3694" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3694" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3694" t="s">
+        <v>3198</v>
+      </c>
+      <c r="E3694" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I3694" t="s">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="3695">
+      <c r="A3695">
+        <v>1765633001</v>
+      </c>
+      <c r="B3695" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3695" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3695" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3695" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3695" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3696">
+      <c r="A3696">
+        <v>1765633001</v>
+      </c>
+      <c r="B3696" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3696" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3696" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3696" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3696" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3697">
+      <c r="A3697">
+        <v>1765633001</v>
+      </c>
+      <c r="B3697" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3697" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3697" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3697" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3697" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3698">
+      <c r="A3698">
+        <v>1765633001</v>
+      </c>
+      <c r="B3698" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3698" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3698" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3698" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3698" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3699">
+      <c r="A3699">
+        <v>1765633001</v>
+      </c>
+      <c r="B3699" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3699" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3699" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3699" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3699" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3700">
+      <c r="A3700">
+        <v>1765633001</v>
+      </c>
+      <c r="B3700" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3700" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3700" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3700" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3700" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3701">
+      <c r="A3701">
+        <v>1765633001</v>
+      </c>
+      <c r="B3701" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3701" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3701" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3701" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3701" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3702">
+      <c r="A3702">
+        <v>1765633001</v>
+      </c>
+      <c r="B3702" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3702" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3702" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3702" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3702" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3703">
+      <c r="A3703">
+        <v>1765633001</v>
+      </c>
+      <c r="B3703" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3703" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3703" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3703" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3703" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3704">
+      <c r="A3704">
+        <v>1765633001</v>
+      </c>
+      <c r="B3704" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3704" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3704" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3704" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3704" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3705">
+      <c r="A3705">
+        <v>1765633001</v>
+      </c>
+      <c r="B3705" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3705" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3705" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3705" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3705" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3706">
+      <c r="A3706">
+        <v>1765633001</v>
+      </c>
+      <c r="B3706" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3706" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3706" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3706" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3706" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3707">
+      <c r="A3707">
+        <v>1765633001</v>
+      </c>
+      <c r="B3707" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3707" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3707" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3707" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3707" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3708">
+      <c r="A3708">
+        <v>1765633001</v>
+      </c>
+      <c r="B3708" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3708" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3708" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3708" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3708" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3709">
+      <c r="A3709">
+        <v>1765633001</v>
+      </c>
+      <c r="B3709" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3709" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3709" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3709" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3709" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>